<commit_message>
Add creditsGiven field to game models and implement credit card assignment script
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931FFF22-C26E-4F99-A2E1-0FCBCAD27EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Teams Data" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Teams Data" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
   <si>
     <t>Team Name</t>
   </si>
@@ -182,7 +178,7 @@
     <t>om, ishan, sahil, parth</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5</t>
+    <t>1, 2, 3, 4, 5, 8, 9, 7, 6</t>
   </si>
   <si>
     <t>MLSC274581924053</t>
@@ -210,27 +206,25 @@
   </si>
   <si>
     <t>Aakarsh, Aryan, Anirudh, Pranav7</t>
+  </si>
+  <si>
+    <t>Reapers</t>
+  </si>
+  <si>
+    <t>Ishwinder, Aradhya, Kumud, Arnav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -253,9 +247,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,48 +587,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H29"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
     <col min="3" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -658,7 +646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -681,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -704,7 +692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -727,7 +715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -750,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -773,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -796,7 +784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -819,7 +807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -842,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -865,7 +853,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -888,7 +876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -911,7 +899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -934,7 +922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -957,7 +945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -980,7 +968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1026,7 +1014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1049,7 +1037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1072,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1118,7 +1106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1141,7 +1129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1167,7 +1155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1190,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1213,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1236,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1259,8 +1247,31 @@
         <v>10</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor user game assignment and update import statements; streamline CORS middleware and add task data structure
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="94">
   <si>
     <t>Team Name</t>
   </si>
@@ -46,132 +46,198 @@
     <t/>
   </si>
   <si>
+    <t>MLSC274581924053</t>
+  </si>
+  <si>
     <t>xantiedar</t>
   </si>
   <si>
     <t>Deb, Tanish Gupta, Achin, Nidhi</t>
   </si>
   <si>
+    <t>MLSC273411206789</t>
+  </si>
+  <si>
     <t>BCS</t>
   </si>
   <si>
     <t>Siddharth, Geet, Yashit Arora, Aryan Thakkar</t>
   </si>
   <si>
+    <t>MLSC278956012348</t>
+  </si>
+  <si>
     <t>Home_Team</t>
   </si>
   <si>
     <t>Akanksha, Hurreet, Jasman, Puranjay</t>
   </si>
   <si>
+    <t>MLSC271900439281</t>
+  </si>
+  <si>
     <t>GajarKaHalwa</t>
   </si>
   <si>
     <t>Harshit, Nikunj Dewan, Tulika, Pranav</t>
   </si>
   <si>
+    <t>MLSC276753908823</t>
+  </si>
+  <si>
     <t>x-tasy</t>
   </si>
   <si>
     <t>Sameer Khan, Karan, Vinesh, Shorya</t>
   </si>
   <si>
+    <t>MLSC278021677349</t>
+  </si>
+  <si>
     <t>BlackHole</t>
   </si>
   <si>
     <t>Tanay, Rohin, Rudra, Krish</t>
   </si>
   <si>
+    <t>MLSC279188325690</t>
+  </si>
+  <si>
     <t>Vanguard</t>
   </si>
   <si>
     <t>Suryansh, Vaibhav, mankirat, Saket</t>
   </si>
   <si>
+    <t>MLSC274012093948</t>
+  </si>
+  <si>
     <t>Andhadun Players</t>
   </si>
   <si>
     <t>Amanjot, Jahanvi, Ram, Dhiren</t>
   </si>
   <si>
+    <t>MLSC273665718204</t>
+  </si>
+  <si>
     <t>BlueBull</t>
   </si>
   <si>
     <t>Shreyansh, Parvesh Lamba, Shriyam, Tanveer</t>
   </si>
   <si>
+    <t>MLSC279937456132</t>
+  </si>
+  <si>
     <t>GenF</t>
   </si>
   <si>
     <t>Piyush, Chirag, Bhagya, Vandini Garg</t>
   </si>
   <si>
+    <t>MLSC275302947685</t>
+  </si>
+  <si>
     <t>Jaguar</t>
   </si>
   <si>
     <t>Anushka Verma, Manvi, Daksh Aggarwal, Uday</t>
   </si>
   <si>
+    <t>MLSC272490411236</t>
+  </si>
+  <si>
     <t>Guns and Roses</t>
   </si>
   <si>
     <t>Prithvi, Sahil, Vrishank, Vani</t>
   </si>
   <si>
+    <t>MLSC278386074821</t>
+  </si>
+  <si>
     <t>Homies</t>
   </si>
   <si>
     <t>Siddhant, Aryan Thakur, Chaitanya, Prerna Garg</t>
   </si>
   <si>
+    <t>MLSC271219486573</t>
+  </si>
+  <si>
     <t>BABLU</t>
   </si>
   <si>
     <t>Vansh, Harsh, Shikhar, Vaibhav Sundriyal</t>
   </si>
   <si>
+    <t>MLSC275630089147</t>
+  </si>
+  <si>
     <t>OUTLAW</t>
   </si>
   <si>
     <t>Arshit, ayush, pragun, aarav</t>
   </si>
   <si>
+    <t>MLSC277953712340</t>
+  </si>
+  <si>
     <t>SQUARE</t>
   </si>
   <si>
     <t>Jasmine, Riya, jyotsna, Anushka</t>
   </si>
   <si>
+    <t>MLSC273519849023</t>
+  </si>
+  <si>
     <t>TSM_entity</t>
   </si>
   <si>
     <t>shounok, amit, aryan, aditya sharma</t>
   </si>
   <si>
+    <t>MLSC272764021980</t>
+  </si>
+  <si>
     <t>Maqsad Returns</t>
   </si>
   <si>
     <t>Yash, Dixant, Ankit Pandey, vrattan</t>
   </si>
   <si>
+    <t>MLSC278241857304</t>
+  </si>
+  <si>
     <t>Syrups</t>
   </si>
   <si>
     <t>Aashish, Abhishek, Ujjwal, Vishesh</t>
   </si>
   <si>
+    <t>MLSC279401358492</t>
+  </si>
+  <si>
     <t>Team Holmes</t>
   </si>
   <si>
     <t>Aayushman, Madhav Gaba, Mahi, hemant</t>
   </si>
   <si>
+    <t>MLSC275146789013</t>
+  </si>
+  <si>
     <t>CRESTFALL</t>
   </si>
   <si>
     <t>Aditya Gupta, Raghav, Aarush, Amish</t>
   </si>
   <si>
+    <t>MLSC273805276149</t>
+  </si>
+  <si>
     <t>IMPOSTORS</t>
   </si>
   <si>
@@ -181,7 +247,7 @@
     <t>1, 2, 3, 4, 5, 8, 9, 7, 6</t>
   </si>
   <si>
-    <t>MLSC274581924053</t>
+    <t>MLSC271729503826</t>
   </si>
   <si>
     <t>Chdi Gang</t>
@@ -190,28 +256,43 @@
     <t>Sameer Verma, Aditya, Vijayshree, Vaibhav Gupta</t>
   </si>
   <si>
+    <t>MLSC276089314578</t>
+  </si>
+  <si>
     <t>Om Rajpal</t>
   </si>
   <si>
     <t>Aman, Angad, Utkal, Kashish</t>
   </si>
   <si>
+    <t>MLSC274920348612</t>
+  </si>
+  <si>
     <t>HR10</t>
   </si>
   <si>
     <t>Sourav, Ishtpreet, Yashkaran, Agrim Bhatt</t>
   </si>
   <si>
+    <t>MLSC273276041398</t>
+  </si>
+  <si>
     <t>Thalaforareason</t>
   </si>
   <si>
     <t>Aakarsh, Aryan, Anirudh, Pranav7</t>
   </si>
   <si>
+    <t>MLSC275490028347</t>
+  </si>
+  <si>
     <t>Reapers</t>
   </si>
   <si>
     <t>Ishwinder, Aradhya, Kumud, Arnav</t>
+  </si>
+  <si>
+    <t>MLSC277150283904</t>
   </si>
 </sst>
 </file>
@@ -623,7 +704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -645,13 +726,16 @@
       <c r="G2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -668,13 +752,16 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -691,13 +778,16 @@
       <c r="G4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -714,13 +804,16 @@
       <c r="G5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -737,13 +830,16 @@
       <c r="G6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -760,13 +856,16 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -783,13 +882,16 @@
       <c r="G8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -806,13 +908,16 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -829,13 +934,16 @@
       <c r="G10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -852,13 +960,16 @@
       <c r="G11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -875,13 +986,16 @@
       <c r="G12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -898,13 +1012,16 @@
       <c r="G13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -921,13 +1038,16 @@
       <c r="G14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -944,13 +1064,16 @@
       <c r="G15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -967,13 +1090,16 @@
       <c r="G16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -990,13 +1116,16 @@
       <c r="G17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1013,13 +1142,16 @@
       <c r="G18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1036,13 +1168,16 @@
       <c r="G19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1059,13 +1194,16 @@
       <c r="G20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1082,13 +1220,16 @@
       <c r="G21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -1105,13 +1246,16 @@
       <c r="G22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -1127,14 +1271,17 @@
       </c>
       <c r="G23" t="s">
         <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
@@ -1149,18 +1296,18 @@
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -1177,13 +1324,16 @@
       <c r="G25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
@@ -1200,13 +1350,16 @@
       <c r="G26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -1223,13 +1376,16 @@
       <c r="G27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -1246,13 +1402,16 @@
       <c r="G28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
@@ -1268,6 +1427,9 @@
       </c>
       <c r="G29" t="s">
         <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove console.log statements for cleaner code; add serial number column in Excel export
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="95">
+  <si>
+    <t>Serial No</t>
+  </si>
   <si>
     <t>Team Name</t>
   </si>
@@ -40,7 +43,7 @@
     <t>Frontslash</t>
   </si>
   <si>
-    <t>Ankush Gautam, Vaibhav Srivastva, Saksham Katna, Aishlee Joshi</t>
+    <t>Ankush Gautam, Vaibhav Srivastva, Mahi, Aishlee Joshi</t>
   </si>
   <si>
     <t/>
@@ -223,7 +226,7 @@
     <t>Team Holmes</t>
   </si>
   <si>
-    <t>Aayushman, Madhav Gaba, Mahi, hemant</t>
+    <t>Aayushman, Madhav Gaba, Saksham Katna, hemant</t>
   </si>
   <si>
     <t>MLSC275146789013</t>
@@ -244,7 +247,7 @@
     <t>om, ishan, sahil, parth</t>
   </si>
   <si>
-    <t>1, 2, 3, 4, 5, 8, 9, 7, 6</t>
+    <t>6, 7, 8</t>
   </si>
   <si>
     <t>MLSC271729503826</t>
@@ -669,16 +672,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,10 +707,13 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -715,721 +722,805 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="I2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="H24" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="I24" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>93</v>
+        <v>11</v>
+      </c>
+      <c r="I29" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update power-up credits and enhance team data structure in Excel export
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="96">
   <si>
     <t>Serial No</t>
   </si>
@@ -40,10 +40,13 @@
     <t>Credit Card No</t>
   </si>
   <si>
+    <t>Score</t>
+  </si>
+  <si>
     <t>Frontslash</t>
   </si>
   <si>
-    <t>Ankush Gautam, Vaibhav Srivastva, Mahi, Aishlee Joshi</t>
+    <t>Ankush Gautam, Vaibhav Srivastva, utkal, Aishlee Joshi</t>
   </si>
   <si>
     <t/>
@@ -256,7 +259,7 @@
     <t>Chdi Gang</t>
   </si>
   <si>
-    <t>Sameer Verma, Aditya, Vijayshree, Vaibhav Gupta</t>
+    <t>Sameer Verma, Aditya, Palak, Vaibhav Gupta</t>
   </si>
   <si>
     <t>MLSC276089314578</t>
@@ -265,7 +268,7 @@
     <t>Om Rajpal</t>
   </si>
   <si>
-    <t>Aman, Angad, Utkal, Kashish</t>
+    <t>Aman, Angad, harshil, Kashish</t>
   </si>
   <si>
     <t>MLSC274920348612</t>
@@ -283,7 +286,7 @@
     <t>Thalaforareason</t>
   </si>
   <si>
-    <t>Aakarsh, Aryan, Anirudh, Pranav7</t>
+    <t>Aakarsh, Aryan2, Anirudh, Pranav7</t>
   </si>
   <si>
     <t>MLSC275490028347</t>
@@ -672,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -680,9 +683,10 @@
     <col min="3" max="3" width="50" customWidth="1"/>
     <col min="4" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,817 +714,904 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="J2">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="J4">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>2930</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J6">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J7">
+        <v>7182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J8">
+        <v>5103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J9">
+        <v>5387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="J10">
+        <v>5935</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="J12">
+        <v>3591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J13">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J14">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="J15">
+        <v>2740</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J16">
+        <v>6898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="J17">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="J19">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="J20">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="J21">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="J22">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="J23">
+        <v>6520</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="J24">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="J25">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="J26">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="J27">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="J28">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="J29">
+        <v>2741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update task data titles and descriptions; enhance power-ups data structure in team routes
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -250,7 +250,7 @@
     <t>om, ishan, sahil, parth</t>
   </si>
   <si>
-    <t>6, 7, 8</t>
+    <t>2, 4, 7, 6</t>
   </si>
   <si>
     <t>MLSC271729503826</t>
@@ -259,7 +259,7 @@
     <t>Chdi Gang</t>
   </si>
   <si>
-    <t>Sameer Verma, Aditya, Palak, Vaibhav Gupta</t>
+    <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
   </si>
   <si>
     <t>MLSC276089314578</t>
@@ -747,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="J2">
-        <v>2835</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>1418</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>7182</v>
+        <v>7282</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>80</v>
       </c>
       <c r="J24">
-        <v>1059</v>
+        <v>454</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add leaderboard route and teams data; refactor answer validation logic
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
   <si>
     <t>Serial No</t>
   </si>
@@ -49,6 +49,18 @@
     <t>Ankush Gautam, Vaibhav Srivastva, utkal, Aishlee Joshi</t>
   </si>
   <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>101, 102, 103, 104, 105</t>
+  </si>
+  <si>
+    <t>201, 202, 203, 204, 205</t>
+  </si>
+  <si>
+    <t>301, 302, 303, 304, 305</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -61,6 +73,18 @@
     <t>Deb, Tanish Gupta, Achin, Nidhi</t>
   </si>
   <si>
+    <t>2, 3, 1</t>
+  </si>
+  <si>
+    <t>102, 103, 104, 105, 101</t>
+  </si>
+  <si>
+    <t>202, 203, 204, 205, 201</t>
+  </si>
+  <si>
+    <t>302, 303, 304, 305, 301</t>
+  </si>
+  <si>
     <t>MLSC273411206789</t>
   </si>
   <si>
@@ -70,6 +94,18 @@
     <t>Siddharth, Geet, Yashit Arora, Aryan Thakkar</t>
   </si>
   <si>
+    <t>3, 1, 2</t>
+  </si>
+  <si>
+    <t>103, 104, 105, 101, 102</t>
+  </si>
+  <si>
+    <t>203, 204, 205, 201, 202</t>
+  </si>
+  <si>
+    <t>303, 304, 305, 301, 302</t>
+  </si>
+  <si>
     <t>MLSC278956012348</t>
   </si>
   <si>
@@ -79,6 +115,15 @@
     <t>Akanksha, Hurreet, Jasman, Puranjay</t>
   </si>
   <si>
+    <t>104, 105, 101, 102, 103</t>
+  </si>
+  <si>
+    <t>204, 205, 201, 202, 203</t>
+  </si>
+  <si>
+    <t>304, 305, 301, 302, 303</t>
+  </si>
+  <si>
     <t>MLSC271900439281</t>
   </si>
   <si>
@@ -88,6 +133,15 @@
     <t>Harshit, Nikunj Dewan, Tulika, Pranav</t>
   </si>
   <si>
+    <t>105, 101, 102, 103, 104</t>
+  </si>
+  <si>
+    <t>205, 201, 202, 203, 204</t>
+  </si>
+  <si>
+    <t>305, 301, 302, 303, 304</t>
+  </si>
+  <si>
     <t>MLSC276753908823</t>
   </si>
   <si>
@@ -178,6 +232,9 @@
     <t>Vansh, Harsh, Shikhar, Vaibhav Sundriyal</t>
   </si>
   <si>
+    <t>5, 2, 7</t>
+  </si>
+  <si>
     <t>MLSC275630089147</t>
   </si>
   <si>
@@ -232,6 +289,9 @@
     <t>Aayushman, Madhav Gaba, Saksham Katna, hemant</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>MLSC275146789013</t>
   </si>
   <si>
@@ -244,61 +304,49 @@
     <t>MLSC273805276149</t>
   </si>
   <si>
-    <t>IMPOSTORS</t>
-  </si>
-  <si>
-    <t>om, ishan, sahil, parth</t>
-  </si>
-  <si>
-    <t>2, 4, 7, 6</t>
+    <t>Chdi Gang</t>
+  </si>
+  <si>
+    <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
   </si>
   <si>
     <t>MLSC271729503826</t>
   </si>
   <si>
-    <t>Chdi Gang</t>
-  </si>
-  <si>
-    <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
+    <t>Om Rajpal</t>
+  </si>
+  <si>
+    <t>Aman, Angad, harshil, Kashish</t>
   </si>
   <si>
     <t>MLSC276089314578</t>
   </si>
   <si>
-    <t>Om Rajpal</t>
-  </si>
-  <si>
-    <t>Aman, Angad, harshil, Kashish</t>
+    <t>HR10</t>
+  </si>
+  <si>
+    <t>Sourav, Ishtpreet, Yashkaran, Agrim Bhatt</t>
   </si>
   <si>
     <t>MLSC274920348612</t>
   </si>
   <si>
-    <t>HR10</t>
-  </si>
-  <si>
-    <t>Sourav, Ishtpreet, Yashkaran, Agrim Bhatt</t>
+    <t>Thalaforareason</t>
+  </si>
+  <si>
+    <t>Aakarsh, Aryan2, Anirudh, Pranav7</t>
   </si>
   <si>
     <t>MLSC273276041398</t>
   </si>
   <si>
-    <t>Thalaforareason</t>
-  </si>
-  <si>
-    <t>Aakarsh, Aryan2, Anirudh, Pranav7</t>
+    <t>Reapers</t>
+  </si>
+  <si>
+    <t>Ishwinder, Aradhya, Kumud, Arnav</t>
   </si>
   <si>
     <t>MLSC275490028347</t>
-  </si>
-  <si>
-    <t>Reapers</t>
-  </si>
-  <si>
-    <t>Ishwinder, Aradhya, Kumud, Arnav</t>
-  </si>
-  <si>
-    <t>MLSC277150283904</t>
   </si>
 </sst>
 </file>
@@ -675,7 +723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -732,19 +780,19 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J2">
         <v>2985</v>
@@ -755,28 +803,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J3">
         <v>1618</v>
@@ -787,28 +835,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="J4">
         <v>3875</v>
@@ -819,28 +867,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>2930</v>
@@ -851,28 +899,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="J6">
         <v>4347</v>
@@ -883,28 +931,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="J7">
         <v>7282</v>
@@ -915,28 +963,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J8">
         <v>5103</v>
@@ -947,28 +995,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="J9">
         <v>5387</v>
@@ -979,28 +1027,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="J10">
         <v>5935</v>
@@ -1011,28 +1059,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="J11">
         <v>2268</v>
@@ -1043,28 +1091,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="J12">
         <v>3591</v>
@@ -1075,28 +1123,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="J13">
         <v>5954</v>
@@ -1107,28 +1155,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="J14">
         <v>2457</v>
@@ -1139,28 +1187,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="J15">
         <v>2740</v>
@@ -1171,31 +1219,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="J16">
-        <v>6898</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1203,28 +1251,28 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="J17">
         <v>1985</v>
@@ -1235,28 +1283,28 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1267,28 +1315,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="J19">
         <v>1985</v>
@@ -1299,28 +1347,28 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H20" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="J20">
         <v>4309</v>
@@ -1331,28 +1379,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="J21">
         <v>3875</v>
@@ -1363,31 +1411,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="J22">
-        <v>2268</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1395,28 +1443,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="J23">
         <v>6520</v>
@@ -1427,31 +1475,31 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="J24">
-        <v>454</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1459,31 +1507,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="J25">
-        <v>3780</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1491,31 +1539,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="J26">
-        <v>3100</v>
+        <v>662</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1523,31 +1571,31 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I27" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="J27">
-        <v>662</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1555,62 +1603,30 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="J28">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I29" t="s">
-        <v>95</v>
-      </c>
-      <c r="J29">
         <v>2741</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix admin login response to include taskId and update hashPassword test case with new input
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
   <si>
     <t>Serial No</t>
   </si>
@@ -43,10 +43,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Frontslash</t>
-  </si>
-  <si>
-    <t>Ankush Gautam, Vaibhav Srivastva, utkal, Aishlee Joshi</t>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t>User1, User2, User3, User4</t>
   </si>
   <si>
     <t>1, 2, 3</t>
@@ -67,10 +67,10 @@
     <t>MLSC274581924053</t>
   </si>
   <si>
-    <t>xantiedar</t>
-  </si>
-  <si>
-    <t>Deb, Tanish Gupta, Achin, Nidhi</t>
+    <t>Team 2</t>
+  </si>
+  <si>
+    <t>User5, User6, User7, User8</t>
   </si>
   <si>
     <t>2, 3, 1</t>
@@ -88,10 +88,10 @@
     <t>MLSC273411206789</t>
   </si>
   <si>
-    <t>BCS</t>
-  </si>
-  <si>
-    <t>Siddharth, Geet, Yashit Arora, Aryan Thakkar</t>
+    <t>Team 3</t>
+  </si>
+  <si>
+    <t>User9, User10, User11, User12</t>
   </si>
   <si>
     <t>3, 1, 2</t>
@@ -109,10 +109,10 @@
     <t>MLSC278956012348</t>
   </si>
   <si>
-    <t>Home_Team</t>
-  </si>
-  <si>
-    <t>Akanksha, Hurreet, Jasman, Puranjay</t>
+    <t>Team 4</t>
+  </si>
+  <si>
+    <t>User13, User14, User15, User16</t>
   </si>
   <si>
     <t>104, 105, 101, 102, 103</t>
@@ -127,10 +127,10 @@
     <t>MLSC271900439281</t>
   </si>
   <si>
-    <t>GajarKaHalwa</t>
-  </si>
-  <si>
-    <t>Harshit, Nikunj Dewan, Tulika, Pranav</t>
+    <t>Team 5</t>
+  </si>
+  <si>
+    <t>User17, User18, User19, User20</t>
   </si>
   <si>
     <t>105, 101, 102, 103, 104</t>
@@ -145,208 +145,139 @@
     <t>MLSC276753908823</t>
   </si>
   <si>
-    <t>x-tasy</t>
-  </si>
-  <si>
-    <t>Sameer Khan, Karan, Vinesh, Shorya</t>
+    <t>Team 6</t>
+  </si>
+  <si>
+    <t>User21, User22, User23, User24</t>
   </si>
   <si>
     <t>MLSC278021677349</t>
   </si>
   <si>
-    <t>BlackHole</t>
-  </si>
-  <si>
-    <t>Tanay, Rohin, Rudra, Krish</t>
+    <t>Team 7</t>
+  </si>
+  <si>
+    <t>User25, User26, User27, User28</t>
   </si>
   <si>
     <t>MLSC279188325690</t>
   </si>
   <si>
-    <t>Vanguard</t>
-  </si>
-  <si>
-    <t>Suryansh, Vaibhav, mankirat, Saket</t>
+    <t>Team 8</t>
+  </si>
+  <si>
+    <t>User29, User30, User31, User32</t>
   </si>
   <si>
     <t>MLSC274012093948</t>
   </si>
   <si>
-    <t>Andhadun Players</t>
-  </si>
-  <si>
-    <t>Amanjot, Jahanvi, Ram, Dhiren</t>
+    <t>Team 9</t>
+  </si>
+  <si>
+    <t>User33, User34, User35, User36</t>
   </si>
   <si>
     <t>MLSC273665718204</t>
   </si>
   <si>
-    <t>BlueBull</t>
-  </si>
-  <si>
-    <t>Shreyansh, Parvesh Lamba, Shriyam, Tanveer</t>
+    <t>Team 10</t>
+  </si>
+  <si>
+    <t>User37, User38, User39, User40</t>
   </si>
   <si>
     <t>MLSC279937456132</t>
   </si>
   <si>
-    <t>GenF</t>
-  </si>
-  <si>
-    <t>Piyush, Chirag, Bhagya, Vandini Garg</t>
+    <t>Team 11</t>
+  </si>
+  <si>
+    <t>User41, User42, User43, User44</t>
   </si>
   <si>
     <t>MLSC275302947685</t>
   </si>
   <si>
-    <t>Jaguar</t>
-  </si>
-  <si>
-    <t>Anushka Verma, Manvi, Daksh Aggarwal, Uday</t>
+    <t>Team 12</t>
+  </si>
+  <si>
+    <t>User45, User46, User47, User48</t>
   </si>
   <si>
     <t>MLSC272490411236</t>
   </si>
   <si>
-    <t>Guns and Roses</t>
-  </si>
-  <si>
-    <t>Prithvi, Sahil, Vrishank, Vani</t>
+    <t>Team 13</t>
+  </si>
+  <si>
+    <t>User49, User50, User51, User52</t>
   </si>
   <si>
     <t>MLSC278386074821</t>
   </si>
   <si>
-    <t>Homies</t>
-  </si>
-  <si>
-    <t>Siddhant, Aryan Thakur, Chaitanya, Prerna Garg</t>
+    <t>Team 14</t>
+  </si>
+  <si>
+    <t>User53, User54, User55, User56</t>
   </si>
   <si>
     <t>MLSC271219486573</t>
   </si>
   <si>
-    <t>BABLU</t>
-  </si>
-  <si>
-    <t>Vansh, Harsh, Shikhar, Vaibhav Sundriyal</t>
-  </si>
-  <si>
-    <t>5, 2, 7</t>
+    <t>Team 15</t>
+  </si>
+  <si>
+    <t>User57, User58, User59, User60</t>
   </si>
   <si>
     <t>MLSC275630089147</t>
   </si>
   <si>
-    <t>OUTLAW</t>
-  </si>
-  <si>
-    <t>Arshit, ayush, pragun, aarav</t>
+    <t>Team 16</t>
+  </si>
+  <si>
+    <t>User61, User62, User63, User64</t>
   </si>
   <si>
     <t>MLSC277953712340</t>
   </si>
   <si>
-    <t>SQUARE</t>
-  </si>
-  <si>
-    <t>Jasmine, Riya, jyotsna, Anushka</t>
+    <t>Team 17</t>
+  </si>
+  <si>
+    <t>User65, User66, User67, User68</t>
   </si>
   <si>
     <t>MLSC273519849023</t>
   </si>
   <si>
-    <t>TSM_entity</t>
-  </si>
-  <si>
-    <t>shounok, amit, aryan, aditya sharma</t>
+    <t>Team 18</t>
+  </si>
+  <si>
+    <t>User69, User70, User71, User72</t>
   </si>
   <si>
     <t>MLSC272764021980</t>
   </si>
   <si>
-    <t>Maqsad Returns</t>
-  </si>
-  <si>
-    <t>Yash, Dixant, Ankit Pandey, vrattan</t>
+    <t>Team 19</t>
+  </si>
+  <si>
+    <t>User73, User74, User75, User76</t>
   </si>
   <si>
     <t>MLSC278241857304</t>
   </si>
   <si>
-    <t>Syrups</t>
-  </si>
-  <si>
-    <t>Aashish, Abhishek, Ujjwal, Vishesh</t>
+    <t>Team 20</t>
+  </si>
+  <si>
+    <t>User77, User78, User79, User80</t>
   </si>
   <si>
     <t>MLSC279401358492</t>
-  </si>
-  <si>
-    <t>Team Holmes</t>
-  </si>
-  <si>
-    <t>Aayushman, Madhav Gaba, Saksham Katna, hemant</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>MLSC275146789013</t>
-  </si>
-  <si>
-    <t>CRESTFALL</t>
-  </si>
-  <si>
-    <t>Aditya Gupta, Raghav, Aarush, Amish</t>
-  </si>
-  <si>
-    <t>MLSC273805276149</t>
-  </si>
-  <si>
-    <t>Chdi Gang</t>
-  </si>
-  <si>
-    <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
-  </si>
-  <si>
-    <t>MLSC271729503826</t>
-  </si>
-  <si>
-    <t>Om Rajpal</t>
-  </si>
-  <si>
-    <t>Aman, Angad, harshil, Kashish</t>
-  </si>
-  <si>
-    <t>MLSC276089314578</t>
-  </si>
-  <si>
-    <t>HR10</t>
-  </si>
-  <si>
-    <t>Sourav, Ishtpreet, Yashkaran, Agrim Bhatt</t>
-  </si>
-  <si>
-    <t>MLSC274920348612</t>
-  </si>
-  <si>
-    <t>Thalaforareason</t>
-  </si>
-  <si>
-    <t>Aakarsh, Aryan2, Anirudh, Pranav7</t>
-  </si>
-  <si>
-    <t>MLSC273276041398</t>
-  </si>
-  <si>
-    <t>Reapers</t>
-  </si>
-  <si>
-    <t>Ishwinder, Aradhya, Kumud, Arnav</t>
-  </si>
-  <si>
-    <t>MLSC275490028347</t>
   </si>
 </sst>
 </file>
@@ -723,7 +654,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -795,7 +726,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>2985</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -827,7 +758,7 @@
         <v>24</v>
       </c>
       <c r="J3">
-        <v>1618</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -859,7 +790,7 @@
         <v>31</v>
       </c>
       <c r="J4">
-        <v>3875</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -891,7 +822,7 @@
         <v>37</v>
       </c>
       <c r="J5">
-        <v>2930</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -923,7 +854,7 @@
         <v>43</v>
       </c>
       <c r="J6">
-        <v>4347</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,7 +886,7 @@
         <v>46</v>
       </c>
       <c r="J7">
-        <v>7282</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -987,7 +918,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>5103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1019,7 +950,7 @@
         <v>52</v>
       </c>
       <c r="J9">
-        <v>5387</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1051,7 +982,7 @@
         <v>55</v>
       </c>
       <c r="J10">
-        <v>5935</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1083,7 +1014,7 @@
         <v>58</v>
       </c>
       <c r="J11">
-        <v>2268</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1115,7 +1046,7 @@
         <v>61</v>
       </c>
       <c r="J12">
-        <v>3591</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1147,7 +1078,7 @@
         <v>64</v>
       </c>
       <c r="J13">
-        <v>5954</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1179,7 +1110,7 @@
         <v>67</v>
       </c>
       <c r="J14">
-        <v>2457</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1211,7 +1142,7 @@
         <v>70</v>
       </c>
       <c r="J15">
-        <v>2740</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1237,13 +1168,13 @@
         <v>42</v>
       </c>
       <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
         <v>73</v>
       </c>
-      <c r="I16" t="s">
-        <v>74</v>
-      </c>
       <c r="J16">
-        <v>401</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1251,10 +1182,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
         <v>75</v>
-      </c>
-      <c r="C17" t="s">
-        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1272,10 +1203,10 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J17">
-        <v>1985</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1283,10 +1214,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
         <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1304,10 +1235,10 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1315,10 +1246,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
         <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -1336,10 +1267,10 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J19">
-        <v>1985</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,10 +1278,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" t="s">
-        <v>85</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1368,10 +1299,10 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J20">
-        <v>4309</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,10 +1310,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
         <v>87</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -1400,234 +1331,10 @@
         <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J21">
-        <v>3875</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" t="s">
-        <v>96</v>
-      </c>
-      <c r="J23">
-        <v>6520</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" t="s">
-        <v>99</v>
-      </c>
-      <c r="J24">
-        <v>3780</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" t="s">
-        <v>105</v>
-      </c>
-      <c r="J26">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" t="s">
-        <v>108</v>
-      </c>
-      <c r="J27">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>109</v>
-      </c>
-      <c r="C28" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J28">
-        <v>2741</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update power-ups and task titles, modify hash password logging, and adjust sample email in registration mail function
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
   <si>
     <t>Serial No</t>
   </si>
@@ -43,10 +43,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Team 1</t>
-  </si>
-  <si>
-    <t>User1, User2, User3, User4</t>
+    <t>Frontslash</t>
+  </si>
+  <si>
+    <t>Ankush Gautam, Vaibhav Srivastva, utkal, Aishlee Joshi</t>
   </si>
   <si>
     <t>1, 2, 3</t>
@@ -67,10 +67,10 @@
     <t>MLSC274581924053</t>
   </si>
   <si>
-    <t>Team 2</t>
-  </si>
-  <si>
-    <t>User5, User6, User7, User8</t>
+    <t>xantiedar</t>
+  </si>
+  <si>
+    <t>Deb, Tanish Gupta, Achin, Nidhi</t>
   </si>
   <si>
     <t>2, 3, 1</t>
@@ -88,10 +88,10 @@
     <t>MLSC273411206789</t>
   </si>
   <si>
-    <t>Team 3</t>
-  </si>
-  <si>
-    <t>User9, User10, User11, User12</t>
+    <t>BCS</t>
+  </si>
+  <si>
+    <t>Siddharth, Geet, Yashit Arora, Aryan Thakkar</t>
   </si>
   <si>
     <t>3, 1, 2</t>
@@ -109,10 +109,10 @@
     <t>MLSC278956012348</t>
   </si>
   <si>
-    <t>Team 4</t>
-  </si>
-  <si>
-    <t>User13, User14, User15, User16</t>
+    <t>Home_Team</t>
+  </si>
+  <si>
+    <t>Akanksha, Hurreet, Jasman, Puranjay</t>
   </si>
   <si>
     <t>104, 105, 101, 102, 103</t>
@@ -127,10 +127,10 @@
     <t>MLSC271900439281</t>
   </si>
   <si>
-    <t>Team 5</t>
-  </si>
-  <si>
-    <t>User17, User18, User19, User20</t>
+    <t>GajarKaHalwa</t>
+  </si>
+  <si>
+    <t>Harshit, Nikunj Dewan, Tulika, Pranav</t>
   </si>
   <si>
     <t>105, 101, 102, 103, 104</t>
@@ -145,139 +145,208 @@
     <t>MLSC276753908823</t>
   </si>
   <si>
-    <t>Team 6</t>
-  </si>
-  <si>
-    <t>User21, User22, User23, User24</t>
+    <t>x-tasy</t>
+  </si>
+  <si>
+    <t>Sameer Khan, Karan, Vinesh, Shorya</t>
   </si>
   <si>
     <t>MLSC278021677349</t>
   </si>
   <si>
-    <t>Team 7</t>
-  </si>
-  <si>
-    <t>User25, User26, User27, User28</t>
+    <t>BlackHole</t>
+  </si>
+  <si>
+    <t>Tanay, Rohin, Rudra, Krish</t>
   </si>
   <si>
     <t>MLSC279188325690</t>
   </si>
   <si>
-    <t>Team 8</t>
-  </si>
-  <si>
-    <t>User29, User30, User31, User32</t>
+    <t>Vanguard</t>
+  </si>
+  <si>
+    <t>Suryansh, Vaibhav, mankirat, Saket</t>
   </si>
   <si>
     <t>MLSC274012093948</t>
   </si>
   <si>
-    <t>Team 9</t>
-  </si>
-  <si>
-    <t>User33, User34, User35, User36</t>
+    <t>Andhadun Players</t>
+  </si>
+  <si>
+    <t>Amanjot, Jahanvi, Ram, Dhiren</t>
   </si>
   <si>
     <t>MLSC273665718204</t>
   </si>
   <si>
-    <t>Team 10</t>
-  </si>
-  <si>
-    <t>User37, User38, User39, User40</t>
+    <t>BlueBull</t>
+  </si>
+  <si>
+    <t>Shreyansh, Parvesh Lamba, Shriyam, Tanveer</t>
   </si>
   <si>
     <t>MLSC279937456132</t>
   </si>
   <si>
-    <t>Team 11</t>
-  </si>
-  <si>
-    <t>User41, User42, User43, User44</t>
+    <t>GenF</t>
+  </si>
+  <si>
+    <t>Piyush, Chirag, Bhagya, Vandini Garg</t>
   </si>
   <si>
     <t>MLSC275302947685</t>
   </si>
   <si>
-    <t>Team 12</t>
-  </si>
-  <si>
-    <t>User45, User46, User47, User48</t>
+    <t>Jaguar</t>
+  </si>
+  <si>
+    <t>Anushka Verma, Manvi, Daksh Aggarwal, Uday</t>
   </si>
   <si>
     <t>MLSC272490411236</t>
   </si>
   <si>
-    <t>Team 13</t>
-  </si>
-  <si>
-    <t>User49, User50, User51, User52</t>
+    <t>Guns and Roses</t>
+  </si>
+  <si>
+    <t>Prithvi, Sahil, Vrishank, Vani</t>
   </si>
   <si>
     <t>MLSC278386074821</t>
   </si>
   <si>
-    <t>Team 14</t>
-  </si>
-  <si>
-    <t>User53, User54, User55, User56</t>
+    <t>Homies</t>
+  </si>
+  <si>
+    <t>Siddhant, Aryan Thakur, Chaitanya, Prerna Garg</t>
   </si>
   <si>
     <t>MLSC271219486573</t>
   </si>
   <si>
-    <t>Team 15</t>
-  </si>
-  <si>
-    <t>User57, User58, User59, User60</t>
+    <t>BABLU</t>
+  </si>
+  <si>
+    <t>Vansh, Harsh, Shikhar, Vaibhav Sundriyal</t>
+  </si>
+  <si>
+    <t>5, 2, 7</t>
   </si>
   <si>
     <t>MLSC275630089147</t>
   </si>
   <si>
-    <t>Team 16</t>
-  </si>
-  <si>
-    <t>User61, User62, User63, User64</t>
+    <t>OUTLAW</t>
+  </si>
+  <si>
+    <t>Arshit, ayush, pragun, aarav</t>
   </si>
   <si>
     <t>MLSC277953712340</t>
   </si>
   <si>
-    <t>Team 17</t>
-  </si>
-  <si>
-    <t>User65, User66, User67, User68</t>
+    <t>SQUARE</t>
+  </si>
+  <si>
+    <t>Jasmine, Riya, jyotsna, Anushka</t>
   </si>
   <si>
     <t>MLSC273519849023</t>
   </si>
   <si>
-    <t>Team 18</t>
-  </si>
-  <si>
-    <t>User69, User70, User71, User72</t>
+    <t>TSM_entity</t>
+  </si>
+  <si>
+    <t>shounok, amit, aryan, aditya sharma</t>
   </si>
   <si>
     <t>MLSC272764021980</t>
   </si>
   <si>
-    <t>Team 19</t>
-  </si>
-  <si>
-    <t>User73, User74, User75, User76</t>
+    <t>Maqsad Returns</t>
+  </si>
+  <si>
+    <t>Yash, Dixant, Ankit Pandey, vrattan</t>
   </si>
   <si>
     <t>MLSC278241857304</t>
   </si>
   <si>
-    <t>Team 20</t>
-  </si>
-  <si>
-    <t>User77, User78, User79, User80</t>
+    <t>Syrups</t>
+  </si>
+  <si>
+    <t>Aashish, Abhishek, Ujjwal, Vishesh</t>
   </si>
   <si>
     <t>MLSC279401358492</t>
+  </si>
+  <si>
+    <t>Team Holmes</t>
+  </si>
+  <si>
+    <t>Aayushman, Madhav Gaba, Saksham Katna, hemant</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>MLSC275146789013</t>
+  </si>
+  <si>
+    <t>CRESTFALL</t>
+  </si>
+  <si>
+    <t>Aditya Gupta, Raghav, Aarush, Amish</t>
+  </si>
+  <si>
+    <t>MLSC273805276149</t>
+  </si>
+  <si>
+    <t>Chdi Gang</t>
+  </si>
+  <si>
+    <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
+  </si>
+  <si>
+    <t>MLSC271729503826</t>
+  </si>
+  <si>
+    <t>Om Rajpal</t>
+  </si>
+  <si>
+    <t>Aman, Angad, harshil, Kashish</t>
+  </si>
+  <si>
+    <t>MLSC276089314578</t>
+  </si>
+  <si>
+    <t>HR10</t>
+  </si>
+  <si>
+    <t>Sourav, Ishtpreet, Yashkaran, Agrim Bhatt</t>
+  </si>
+  <si>
+    <t>MLSC274920348612</t>
+  </si>
+  <si>
+    <t>Thalaforareason</t>
+  </si>
+  <si>
+    <t>Aakarsh, Aryan2, Anirudh, Pranav7</t>
+  </si>
+  <si>
+    <t>MLSC273276041398</t>
+  </si>
+  <si>
+    <t>Reapers</t>
+  </si>
+  <si>
+    <t>Ishwinder, Aradhya, Kumud, Arnav</t>
+  </si>
+  <si>
+    <t>MLSC275490028347</t>
   </si>
 </sst>
 </file>
@@ -654,7 +723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J28"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -726,7 +795,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -758,7 +827,7 @@
         <v>24</v>
       </c>
       <c r="J3">
-        <v>100</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -790,7 +859,7 @@
         <v>31</v>
       </c>
       <c r="J4">
-        <v>100</v>
+        <v>3875</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -822,7 +891,7 @@
         <v>37</v>
       </c>
       <c r="J5">
-        <v>100</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -854,7 +923,7 @@
         <v>43</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -886,7 +955,7 @@
         <v>46</v>
       </c>
       <c r="J7">
-        <v>100</v>
+        <v>7282</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -918,7 +987,7 @@
         <v>49</v>
       </c>
       <c r="J8">
-        <v>100</v>
+        <v>5103</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -950,7 +1019,7 @@
         <v>52</v>
       </c>
       <c r="J9">
-        <v>100</v>
+        <v>5387</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,7 +1051,7 @@
         <v>55</v>
       </c>
       <c r="J10">
-        <v>100</v>
+        <v>5935</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1014,7 +1083,7 @@
         <v>58</v>
       </c>
       <c r="J11">
-        <v>100</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1046,7 +1115,7 @@
         <v>61</v>
       </c>
       <c r="J12">
-        <v>100</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1078,7 +1147,7 @@
         <v>64</v>
       </c>
       <c r="J13">
-        <v>100</v>
+        <v>5954</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1110,7 +1179,7 @@
         <v>67</v>
       </c>
       <c r="J14">
-        <v>100</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1142,7 +1211,7 @@
         <v>70</v>
       </c>
       <c r="J15">
-        <v>100</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,13 +1237,13 @@
         <v>42</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J16">
-        <v>100</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1182,10 +1251,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1203,10 +1272,10 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J17">
-        <v>100</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1214,10 +1283,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1235,10 +1304,10 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J18">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1246,10 +1315,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -1267,10 +1336,10 @@
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J19">
-        <v>100</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1278,10 +1347,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1299,10 +1368,10 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J20">
-        <v>100</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1310,10 +1379,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -1331,10 +1400,234 @@
         <v>16</v>
       </c>
       <c r="I21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J21">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23">
+        <v>6520</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24">
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" t="s">
+        <v>108</v>
+      </c>
+      <c r="J27">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28">
+        <v>2741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove commented-out logging for authorization header in request handler
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
   <si>
     <t>Serial No</t>
   </si>
@@ -61,30 +61,33 @@
     <t>301, 302, 303, 304, 305</t>
   </si>
   <si>
+    <t>1, 6, 7</t>
+  </si>
+  <si>
+    <t>MLSC274581924053</t>
+  </si>
+  <si>
+    <t>xantiedar</t>
+  </si>
+  <si>
+    <t>Deb, Tanish Gupta, Achin, Nidhi</t>
+  </si>
+  <si>
+    <t>2, 3, 1</t>
+  </si>
+  <si>
+    <t>102, 103, 104, 105, 101</t>
+  </si>
+  <si>
+    <t>202, 203, 204, 205, 201</t>
+  </si>
+  <si>
+    <t>302, 303, 304, 305, 301</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>MLSC274581924053</t>
-  </si>
-  <si>
-    <t>xantiedar</t>
-  </si>
-  <si>
-    <t>Deb, Tanish Gupta, Achin, Nidhi</t>
-  </si>
-  <si>
-    <t>2, 3, 1</t>
-  </si>
-  <si>
-    <t>102, 103, 104, 105, 101</t>
-  </si>
-  <si>
-    <t>202, 203, 204, 205, 201</t>
-  </si>
-  <si>
-    <t>302, 303, 304, 305, 301</t>
-  </si>
-  <si>
     <t>MLSC273411206789</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
     <t>303, 304, 305, 301, 302</t>
   </si>
   <si>
+    <t>6, 7, 1, 4</t>
+  </si>
+  <si>
     <t>MLSC278956012348</t>
   </si>
   <si>
@@ -124,6 +130,9 @@
     <t>304, 305, 301, 302, 303</t>
   </si>
   <si>
+    <t>1, 6</t>
+  </si>
+  <si>
     <t>MLSC271900439281</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
     <t>305, 301, 302, 303, 304</t>
   </si>
   <si>
+    <t>1, 6, 2</t>
+  </si>
+  <si>
     <t>MLSC276753908823</t>
   </si>
   <si>
@@ -151,6 +163,9 @@
     <t>Sameer Khan, Karan, Vinesh, Shorya</t>
   </si>
   <si>
+    <t>5, 2, 6</t>
+  </si>
+  <si>
     <t>MLSC278021677349</t>
   </si>
   <si>
@@ -169,6 +184,9 @@
     <t>Suryansh, Vaibhav, mankirat, Saket</t>
   </si>
   <si>
+    <t>1, 5</t>
+  </si>
+  <si>
     <t>MLSC274012093948</t>
   </si>
   <si>
@@ -178,6 +196,9 @@
     <t>Amanjot, Jahanvi, Ram, Dhiren</t>
   </si>
   <si>
+    <t>7, 1, 5</t>
+  </si>
+  <si>
     <t>MLSC273665718204</t>
   </si>
   <si>
@@ -187,6 +208,9 @@
     <t>Shreyansh, Parvesh Lamba, Shriyam, Tanveer</t>
   </si>
   <si>
+    <t>6, 7</t>
+  </si>
+  <si>
     <t>MLSC279937456132</t>
   </si>
   <si>
@@ -205,6 +229,9 @@
     <t>Anushka Verma, Manvi, Daksh Aggarwal, Uday</t>
   </si>
   <si>
+    <t>2, 5</t>
+  </si>
+  <si>
     <t>MLSC272490411236</t>
   </si>
   <si>
@@ -262,6 +289,9 @@
     <t>shounok, amit, aryan, aditya sharma</t>
   </si>
   <si>
+    <t>7, 1</t>
+  </si>
+  <si>
     <t>MLSC272764021980</t>
   </si>
   <si>
@@ -271,6 +301,9 @@
     <t>Yash, Dixant, Ankit Pandey, vrattan</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>MLSC278241857304</t>
   </si>
   <si>
@@ -299,6 +332,9 @@
   </si>
   <si>
     <t>Aditya Gupta, Raghav, Aarush, Amish</t>
+  </si>
+  <si>
+    <t>7, 5, 2</t>
   </si>
   <si>
     <t>MLSC273805276149</t>
@@ -795,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="J2">
-        <v>2985</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -821,10 +857,10 @@
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3">
         <v>1618</v>
@@ -835,31 +871,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4">
-        <v>3875</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -867,31 +903,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J5">
-        <v>2930</v>
+        <v>682</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -899,31 +935,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J6">
-        <v>4347</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -931,13 +967,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -949,13 +985,13 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J7">
-        <v>7282</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -963,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -981,10 +1017,10 @@
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="J8">
         <v>5103</v>
@@ -995,31 +1031,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="J9">
-        <v>5387</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,31 +1063,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="J10">
-        <v>5935</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1059,31 +1095,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="J11">
-        <v>2268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1091,10 +1127,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1112,10 +1148,10 @@
         <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="J12">
-        <v>3591</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1123,13 +1159,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>21</v>
@@ -1141,13 +1177,13 @@
         <v>23</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="J13">
-        <v>5954</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1155,28 +1191,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="J14">
         <v>2457</v>
@@ -1187,28 +1223,28 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="J15">
         <v>2740</v>
@@ -1219,28 +1255,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J16">
         <v>401</v>
@@ -1251,10 +1287,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1269,10 +1305,10 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="J17">
         <v>1985</v>
@@ -1283,10 +1319,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -1301,10 +1337,10 @@
         <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1315,31 +1351,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="J19">
-        <v>1985</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,31 +1383,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="J20">
-        <v>4309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,28 +1415,28 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="J21">
         <v>3875</v>
@@ -1411,13 +1447,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -1429,10 +1465,10 @@
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="J22">
         <v>369</v>
@@ -1443,10 +1479,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1461,13 +1497,13 @@
         <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="I23" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="J23">
-        <v>6520</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1475,28 +1511,28 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="J24">
         <v>3780</v>
@@ -1507,28 +1543,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="J25">
         <v>3100</v>
@@ -1539,28 +1575,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="J26">
         <v>662</v>
@@ -1571,10 +1607,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
@@ -1589,13 +1625,13 @@
         <v>15</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="I27" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="J27">
-        <v>2169</v>
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1603,13 +1639,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
@@ -1621,10 +1657,10 @@
         <v>23</v>
       </c>
       <c r="H28" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="J28">
         <v>2741</v>

</xml_diff>

<commit_message>
Comment out powerups patch route in team routes for future reference
</commit_message>
<xml_diff>
--- a/teams_data.xlsx
+++ b/teams_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="125">
   <si>
     <t>Serial No</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>Sameer Verma, Aditya, Palak, Bhavninder</t>
+  </si>
+  <si>
+    <t>8, 7</t>
   </si>
   <si>
     <t>MLSC271729503826</t>
@@ -1529,13 +1532,13 @@
         <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="I24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J24">
-        <v>3780</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1543,10 +1546,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -1564,7 +1567,7 @@
         <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J25">
         <v>3100</v>
@@ -1575,10 +1578,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1596,7 +1599,7 @@
         <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J26">
         <v>662</v>
@@ -1607,10 +1610,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
@@ -1628,7 +1631,7 @@
         <v>92</v>
       </c>
       <c r="I27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J27">
         <v>521</v>
@@ -1639,10 +1642,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -1660,7 +1663,7 @@
         <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J28">
         <v>2741</v>

</xml_diff>